<commit_message>
Move stages of production one level down
</commit_message>
<xml_diff>
--- a/tables/createAutarky.xlsx
+++ b/tables/createAutarky.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1390" uniqueCount="885">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2431" uniqueCount="1548">
   <si>
     <t>Row</t>
   </si>
@@ -2362,6 +2362,1995 @@
   </si>
   <si>
     <t>xi_y2</t>
+  </si>
+  <si>
+    <t>alpha</t>
+  </si>
+  <si>
+    <t>gamma_xx</t>
+  </si>
+  <si>
+    <t>theta</t>
+  </si>
+  <si>
+    <t>zeta_e</t>
+  </si>
+  <si>
+    <t>ss_dg_to_ngdp</t>
+  </si>
+  <si>
+    <t>ss_ncg_to_ngdp</t>
+  </si>
+  <si>
+    <t>tau_cg</t>
+  </si>
+  <si>
+    <t>tau_txl1</t>
+  </si>
+  <si>
+    <t>rho_cg</t>
+  </si>
+  <si>
+    <t>rho_txl2</t>
+  </si>
+  <si>
+    <t>rho_txl1</t>
+  </si>
+  <si>
+    <t>gg_rho_a</t>
+  </si>
+  <si>
+    <t>gg_ss_roc_a</t>
+  </si>
+  <si>
+    <t>gg_rho_nn</t>
+  </si>
+  <si>
+    <t>gg_ss_roc_nn</t>
+  </si>
+  <si>
+    <t>ttrend</t>
+  </si>
+  <si>
+    <t>SteadyLevel</t>
+  </si>
+  <si>
+    <t>SteadyChange</t>
+  </si>
+  <si>
+    <t>Form</t>
+  </si>
+  <si>
+    <t>Rate/</t>
+  </si>
+  <si>
+    <t>Diff-</t>
+  </si>
+  <si>
+    <t>Rate/</t>
+  </si>
+  <si>
+    <t>Diff-</t>
+  </si>
+  <si>
+    <t>Rate/</t>
+  </si>
+  <si>
+    <t>Diff-</t>
+  </si>
+  <si>
+    <t>Rate/</t>
+  </si>
+  <si>
+    <t>Diff-</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Total Population</t>
+  </si>
+  <si>
+    <t>Total Population Relative to Global Population Component</t>
+  </si>
+  <si>
+    <t>Working Age Population</t>
+  </si>
+  <si>
+    <t>Labor Force</t>
+  </si>
+  <si>
+    <t>Real Discount Factor</t>
+  </si>
+  <si>
+    <t>Private Consumption</t>
+  </si>
+  <si>
+    <t>Private Consumption, Point of Reference</t>
+  </si>
+  <si>
+    <t>Per-Capita Labor Supply</t>
+  </si>
+  <si>
+    <t>Variable Labor</t>
+  </si>
+  <si>
+    <t>Private Investment</t>
+  </si>
+  <si>
+    <t>Production Capital</t>
+  </si>
+  <si>
+    <t>Production Capital, Point of Reference</t>
+  </si>
+  <si>
+    <t>Production Capital Services</t>
+  </si>
+  <si>
+    <t>Household Net Worth</t>
+  </si>
+  <si>
+    <t>Domestic Technology Level</t>
+  </si>
+  <si>
+    <t>Shadow Value of Household Budget Constraing</t>
+  </si>
+  <si>
+    <t>Price of Private Consumption</t>
+  </si>
+  <si>
+    <t>Price of Private Investment</t>
+  </si>
+  <si>
+    <t>Roundabout Production</t>
+  </si>
+  <si>
+    <t>Stage T-2 Output</t>
+  </si>
+  <si>
+    <t>Stage T-1 Output</t>
+  </si>
+  <si>
+    <t>Stage T-0 Output</t>
+  </si>
+  <si>
+    <t>Price of Stage T-0 Output</t>
+  </si>
+  <si>
+    <t>Price of State T-1 Output</t>
+  </si>
+  <si>
+    <t>price of Stage T-2 Output</t>
+  </si>
+  <si>
+    <t>Nominal GDP</t>
+  </si>
+  <si>
+    <t>Price of Domestic Production</t>
+  </si>
+  <si>
+    <t>Price of Production Capital</t>
+  </si>
+  <si>
+    <t>Price of Production Capital Services</t>
+  </si>
+  <si>
+    <t>Nominal Wage Rate</t>
+  </si>
+  <si>
+    <t>Nominal Local Currency Money Market Rate</t>
+  </si>
+  <si>
+    <t>Nominal Local Currency Household Lending Rate</t>
+  </si>
+  <si>
+    <t>Bank Deposits</t>
+  </si>
+  <si>
+    <t>Price of Final Domestic Output, Rate of Change</t>
+  </si>
+  <si>
+    <t>Price of Final Domestic Output, Rate of Change, Point of Reference</t>
+  </si>
+  <si>
+    <t>Nominal Wage Rate, Rate of Change</t>
+  </si>
+  <si>
+    <t>Price of Consumer Goods, Rate of Change</t>
+  </si>
+  <si>
+    <t>Household Investment, Rate of Change</t>
+  </si>
+  <si>
+    <t>Capital Utilization Rate</t>
+  </si>
+  <si>
+    <t>Household Capital, Rate of Change</t>
+  </si>
+  <si>
+    <t>Domestic Component of Private Consumption</t>
+  </si>
+  <si>
+    <t>Domestic Component of Government Consumption</t>
+  </si>
+  <si>
+    <t>Domestic Component of Private Investment</t>
+  </si>
+  <si>
+    <t>Total Non-Commodity Imports</t>
+  </si>
+  <si>
+    <t>Price of Imports</t>
+  </si>
+  <si>
+    <t>Import Content of Non-Commodity Exports</t>
+  </si>
+  <si>
+    <t>Intermediate Import Inputs into Domestic Production</t>
+  </si>
+  <si>
+    <t>Domestic Content of Non-Commodity Exports</t>
+  </si>
+  <si>
+    <t>Non-Commodity Exports</t>
+  </si>
+  <si>
+    <t>Price of Non-Commodity Exports</t>
+  </si>
+  <si>
+    <t>Net Foreign Assets to GDP Ratio</t>
+  </si>
+  <si>
+    <t>Effective Interest Rate and Valuation on NFA</t>
+  </si>
+  <si>
+    <t>Checksum for Net Foreign Assets to GDP Ratio</t>
+  </si>
+  <si>
+    <t>Nominal Exchange Rate</t>
+  </si>
+  <si>
+    <t>Expectations of Nominal Exchange Rate</t>
+  </si>
+  <si>
+    <t>Nominal Exchange Rate, Rate of Change</t>
+  </si>
+  <si>
+    <t>Government Debt Interest Rate</t>
+  </si>
+  <si>
+    <t>Price of Government Consumption</t>
+  </si>
+  <si>
+    <t>Government Consumption</t>
+  </si>
+  <si>
+    <t>Government Debt to GDP Ratio</t>
+  </si>
+  <si>
+    <t>Net Lump-Sum Tax Rate on Wealthy Consumers</t>
+  </si>
+  <si>
+    <t>Net Lump-Sum Tax Rate on Poor Consumers</t>
+  </si>
+  <si>
+    <t>Government Consumption, Rate of Change</t>
+  </si>
+  <si>
+    <t>S/S Population, Relative to Global Population Component</t>
+  </si>
+  <si>
+    <t>S/S Share of Working Age Population in Total Population</t>
+  </si>
+  <si>
+    <t>S/S Labor Participation Rate</t>
+  </si>
+  <si>
+    <t>Autoregression in Total Population Relative to Global Population Component</t>
+  </si>
+  <si>
+    <t>Autoregression in Share of Working Age Population in Total Population</t>
+  </si>
+  <si>
+    <t>Autoregression in Labor Participation Rate</t>
+  </si>
+  <si>
+    <t>Import Intensity of Non-Commodity Exports</t>
+  </si>
+  <si>
+    <t>Acceleration in Exportable Productivity</t>
+  </si>
+  <si>
+    <t>Elasticity of Household Lending Rate to Risk</t>
+  </si>
+  <si>
+    <t>Weight on Model-Consistent Expectations in Exchange Rate</t>
+  </si>
+  <si>
+    <t>Time trend</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>nn</t>
+  </si>
+  <si>
+    <t>nr</t>
+  </si>
+  <si>
+    <t>nw</t>
+  </si>
+  <si>
+    <t>nf</t>
+  </si>
+  <si>
+    <t>rdf</t>
+  </si>
+  <si>
+    <t>ch</t>
+  </si>
+  <si>
+    <t>ref_ch</t>
+  </si>
+  <si>
+    <t>nh</t>
+  </si>
+  <si>
+    <t>nv</t>
+  </si>
+  <si>
+    <t>ih</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>ref_k</t>
+  </si>
+  <si>
+    <t>uk</t>
+  </si>
+  <si>
+    <t>netw</t>
+  </si>
+  <si>
+    <t>ar</t>
+  </si>
+  <si>
+    <t>vh</t>
+  </si>
+  <si>
+    <t>pch</t>
+  </si>
+  <si>
+    <t>pih</t>
+  </si>
+  <si>
+    <t>z</t>
+  </si>
+  <si>
+    <t>y2</t>
+  </si>
+  <si>
+    <t>y1</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>py0</t>
+  </si>
+  <si>
+    <t>py1</t>
+  </si>
+  <si>
+    <t>py2</t>
+  </si>
+  <si>
+    <t>ngdp</t>
+  </si>
+  <si>
+    <t>py</t>
+  </si>
+  <si>
+    <t>pk</t>
+  </si>
+  <si>
+    <t>puk</t>
+  </si>
+  <si>
+    <t>w</t>
+  </si>
+  <si>
+    <t>w0</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>rbl</t>
+  </si>
+  <si>
+    <t>bd</t>
+  </si>
+  <si>
+    <t>roc_py</t>
+  </si>
+  <si>
+    <t>ref_roc_py</t>
+  </si>
+  <si>
+    <t>roc_w</t>
+  </si>
+  <si>
+    <t>roc_pch</t>
+  </si>
+  <si>
+    <t>roc_ih</t>
+  </si>
+  <si>
+    <t>u</t>
+  </si>
+  <si>
+    <t>roc_k</t>
+  </si>
+  <si>
+    <t>ych</t>
+  </si>
+  <si>
+    <t>ycg</t>
+  </si>
+  <si>
+    <t>yih</t>
+  </si>
+  <si>
+    <t>mm</t>
+  </si>
+  <si>
+    <t>pmm</t>
+  </si>
+  <si>
+    <t>mxx</t>
+  </si>
+  <si>
+    <t>my</t>
+  </si>
+  <si>
+    <t>yxx</t>
+  </si>
+  <si>
+    <t>xx</t>
+  </si>
+  <si>
+    <t>pxx</t>
+  </si>
+  <si>
+    <t>nfa_to_ngdp</t>
+  </si>
+  <si>
+    <t>rnfa</t>
+  </si>
+  <si>
+    <t>nfa_to_ngdp_checksum</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>exp_e</t>
+  </si>
+  <si>
+    <t>roc_e</t>
+  </si>
+  <si>
+    <t>rg</t>
+  </si>
+  <si>
+    <t>pcg</t>
+  </si>
+  <si>
+    <t>cg</t>
+  </si>
+  <si>
+    <t>dg_to_ngdp</t>
+  </si>
+  <si>
+    <t>txl1</t>
+  </si>
+  <si>
+    <t>txl2</t>
+  </si>
+  <si>
+    <t>roc_cg</t>
+  </si>
+  <si>
+    <t>gg_a</t>
+  </si>
+  <si>
+    <t>gg_nn</t>
+  </si>
+  <si>
+    <t>shk_nr</t>
+  </si>
+  <si>
+    <t>shk_nw_to_nn</t>
+  </si>
+  <si>
+    <t>shk_nf_to_nw</t>
+  </si>
+  <si>
+    <t>shk_ar</t>
+  </si>
+  <si>
+    <t>shk_r</t>
+  </si>
+  <si>
+    <t>shk_w</t>
+  </si>
+  <si>
+    <t>shk_curr</t>
+  </si>
+  <si>
+    <t>shk_cg</t>
+  </si>
+  <si>
+    <t>shk_txl1</t>
+  </si>
+  <si>
+    <t>shk_txl2</t>
+  </si>
+  <si>
+    <t>gg_shk_a</t>
+  </si>
+  <si>
+    <t>gg_shk_nn</t>
+  </si>
+  <si>
+    <t>ss_nr</t>
+  </si>
+  <si>
+    <t>ss_nw_to_nn</t>
+  </si>
+  <si>
+    <t>ss_nf_to_nw</t>
+  </si>
+  <si>
+    <t>rho_nr</t>
+  </si>
+  <si>
+    <t>rho_nw</t>
+  </si>
+  <si>
+    <t>rho_nf</t>
+  </si>
+  <si>
+    <t>rho_ar</t>
+  </si>
+  <si>
+    <t>chi_curr</t>
+  </si>
+  <si>
+    <t>chi_ch</t>
+  </si>
+  <si>
+    <t>chi</t>
+  </si>
+  <si>
+    <t>nu_0</t>
+  </si>
+  <si>
+    <t>nu_1</t>
+  </si>
+  <si>
+    <t>xi_k</t>
+  </si>
+  <si>
+    <t>xi_ih</t>
+  </si>
+  <si>
+    <t>upsilon_0</t>
+  </si>
+  <si>
+    <t>upsilon_1</t>
+  </si>
+  <si>
+    <t>beta</t>
+  </si>
+  <si>
+    <t>beta_k</t>
+  </si>
+  <si>
+    <t>delta</t>
+  </si>
+  <si>
+    <t>gamma_n0</t>
+  </si>
+  <si>
+    <t>gamma_n</t>
+  </si>
+  <si>
+    <t>gamma_uk</t>
+  </si>
+  <si>
+    <t>gamma_z</t>
+  </si>
+  <si>
+    <t>eta</t>
+  </si>
+  <si>
+    <t>rho_w</t>
+  </si>
+  <si>
+    <t>kappa_1</t>
+  </si>
+  <si>
+    <t>kappa_2</t>
+  </si>
+  <si>
+    <t>ss_ar</t>
+  </si>
+  <si>
+    <t>ss_roc_pch</t>
+  </si>
+  <si>
+    <t>xi_py</t>
+  </si>
+  <si>
+    <t>mu_py</t>
+  </si>
+  <si>
+    <t>mu_y2</t>
+  </si>
+  <si>
+    <t>rho_r</t>
+  </si>
+  <si>
+    <t>psi_pch</t>
+  </si>
+  <si>
+    <t>zeta_py</t>
+  </si>
+  <si>
+    <t>xi_ch0</t>
+  </si>
+  <si>
+    <t>xi_ch1</t>
+  </si>
+  <si>
+    <t>xi_ch2</t>
+  </si>
+  <si>
+    <t>xi_y1</t>
+  </si>
+  <si>
+    <t>xi_y2</t>
+  </si>
+  <si>
+    <t>alpha</t>
+  </si>
+  <si>
+    <t>gamma_xx</t>
+  </si>
+  <si>
+    <t>theta</t>
+  </si>
+  <si>
+    <t>zeta_e</t>
+  </si>
+  <si>
+    <t>ss_dg_to_ngdp</t>
+  </si>
+  <si>
+    <t>ss_ncg_to_ngdp</t>
+  </si>
+  <si>
+    <t>tau_cg</t>
+  </si>
+  <si>
+    <t>tau_txl1</t>
+  </si>
+  <si>
+    <t>rho_cg</t>
+  </si>
+  <si>
+    <t>rho_txl2</t>
+  </si>
+  <si>
+    <t>rho_txl1</t>
+  </si>
+  <si>
+    <t>gg_rho_a</t>
+  </si>
+  <si>
+    <t>gg_ss_roc_a</t>
+  </si>
+  <si>
+    <t>gg_rho_nn</t>
+  </si>
+  <si>
+    <t>gg_ss_roc_nn</t>
+  </si>
+  <si>
+    <t>ttrend</t>
+  </si>
+  <si>
+    <t>SteadyLevel</t>
+  </si>
+  <si>
+    <t>SteadyChange</t>
+  </si>
+  <si>
+    <t>Form</t>
+  </si>
+  <si>
+    <t>Rate/</t>
+  </si>
+  <si>
+    <t>Diff-</t>
+  </si>
+  <si>
+    <t>Rate/</t>
+  </si>
+  <si>
+    <t>Diff-</t>
+  </si>
+  <si>
+    <t>Rate/</t>
+  </si>
+  <si>
+    <t>Diff-</t>
+  </si>
+  <si>
+    <t>Rate/</t>
+  </si>
+  <si>
+    <t>Diff-</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Total Population</t>
+  </si>
+  <si>
+    <t>Total Population Relative to Global Population Component</t>
+  </si>
+  <si>
+    <t>Working Age Population</t>
+  </si>
+  <si>
+    <t>Labor Force</t>
+  </si>
+  <si>
+    <t>Real Discount Factor</t>
+  </si>
+  <si>
+    <t>Private Consumption</t>
+  </si>
+  <si>
+    <t>Private Consumption, Point of Reference</t>
+  </si>
+  <si>
+    <t>Per-Capita Labor Supply</t>
+  </si>
+  <si>
+    <t>Variable Labor</t>
+  </si>
+  <si>
+    <t>Private Investment</t>
+  </si>
+  <si>
+    <t>Production Capital</t>
+  </si>
+  <si>
+    <t>Production Capital, Point of Reference</t>
+  </si>
+  <si>
+    <t>Production Capital Services</t>
+  </si>
+  <si>
+    <t>Household Net Worth</t>
+  </si>
+  <si>
+    <t>Domestic Technology Level</t>
+  </si>
+  <si>
+    <t>Shadow Value of Household Budget Constraing</t>
+  </si>
+  <si>
+    <t>Price of Private Consumption</t>
+  </si>
+  <si>
+    <t>Price of Private Investment</t>
+  </si>
+  <si>
+    <t>Roundabout Production</t>
+  </si>
+  <si>
+    <t>Stage T-2 Output</t>
+  </si>
+  <si>
+    <t>Stage T-1 Output</t>
+  </si>
+  <si>
+    <t>Stage T-0 Output</t>
+  </si>
+  <si>
+    <t>Price of Stage T-0 Output</t>
+  </si>
+  <si>
+    <t>Price of State T-1 Output</t>
+  </si>
+  <si>
+    <t>price of Stage T-2 Output</t>
+  </si>
+  <si>
+    <t>Nominal GDP</t>
+  </si>
+  <si>
+    <t>Price of Domestic Production</t>
+  </si>
+  <si>
+    <t>Price of Production Capital</t>
+  </si>
+  <si>
+    <t>Price of Production Capital Services</t>
+  </si>
+  <si>
+    <t>Nominal Wage Rate</t>
+  </si>
+  <si>
+    <t>Nominal Local Currency Money Market Rate</t>
+  </si>
+  <si>
+    <t>Nominal Local Currency Household Lending Rate</t>
+  </si>
+  <si>
+    <t>Bank Deposits</t>
+  </si>
+  <si>
+    <t>Price of Final Domestic Output, Rate of Change</t>
+  </si>
+  <si>
+    <t>Price of Final Domestic Output, Rate of Change, Point of Reference</t>
+  </si>
+  <si>
+    <t>Nominal Wage Rate, Rate of Change</t>
+  </si>
+  <si>
+    <t>Price of Consumer Goods, Rate of Change</t>
+  </si>
+  <si>
+    <t>Household Investment, Rate of Change</t>
+  </si>
+  <si>
+    <t>Capital Utilization Rate</t>
+  </si>
+  <si>
+    <t>Household Capital, Rate of Change</t>
+  </si>
+  <si>
+    <t>Domestic Component of Private Consumption</t>
+  </si>
+  <si>
+    <t>Domestic Component of Government Consumption</t>
+  </si>
+  <si>
+    <t>Domestic Component of Private Investment</t>
+  </si>
+  <si>
+    <t>Total Non-Commodity Imports</t>
+  </si>
+  <si>
+    <t>Price of Imports</t>
+  </si>
+  <si>
+    <t>Import Content of Non-Commodity Exports</t>
+  </si>
+  <si>
+    <t>Intermediate Import Inputs into Domestic Production</t>
+  </si>
+  <si>
+    <t>Domestic Content of Non-Commodity Exports</t>
+  </si>
+  <si>
+    <t>Non-Commodity Exports</t>
+  </si>
+  <si>
+    <t>Price of Non-Commodity Exports</t>
+  </si>
+  <si>
+    <t>Net Foreign Assets to GDP Ratio</t>
+  </si>
+  <si>
+    <t>Effective Interest Rate and Valuation on NFA</t>
+  </si>
+  <si>
+    <t>Checksum for Net Foreign Assets to GDP Ratio</t>
+  </si>
+  <si>
+    <t>Nominal Exchange Rate</t>
+  </si>
+  <si>
+    <t>Expectations of Nominal Exchange Rate</t>
+  </si>
+  <si>
+    <t>Nominal Exchange Rate, Rate of Change</t>
+  </si>
+  <si>
+    <t>Government Debt Interest Rate</t>
+  </si>
+  <si>
+    <t>Price of Government Consumption</t>
+  </si>
+  <si>
+    <t>Government Consumption</t>
+  </si>
+  <si>
+    <t>Government Debt to GDP Ratio</t>
+  </si>
+  <si>
+    <t>Net Lump-Sum Tax Rate on Wealthy Consumers</t>
+  </si>
+  <si>
+    <t>Net Lump-Sum Tax Rate on Poor Consumers</t>
+  </si>
+  <si>
+    <t>Government Consumption, Rate of Change</t>
+  </si>
+  <si>
+    <t>S/S Population, Relative to Global Population Component</t>
+  </si>
+  <si>
+    <t>S/S Share of Working Age Population in Total Population</t>
+  </si>
+  <si>
+    <t>S/S Labor Participation Rate</t>
+  </si>
+  <si>
+    <t>Autoregression in Total Population Relative to Global Population Component</t>
+  </si>
+  <si>
+    <t>Autoregression in Share of Working Age Population in Total Population</t>
+  </si>
+  <si>
+    <t>Autoregression in Labor Participation Rate</t>
+  </si>
+  <si>
+    <t>Import Intensity of Non-Commodity Exports</t>
+  </si>
+  <si>
+    <t>Acceleration in Exportable Productivity</t>
+  </si>
+  <si>
+    <t>Elasticity of Household Lending Rate to Risk</t>
+  </si>
+  <si>
+    <t>Weight on Model-Consistent Expectations in Exchange Rate</t>
+  </si>
+  <si>
+    <t>Time trend</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>nn</t>
+  </si>
+  <si>
+    <t>nr</t>
+  </si>
+  <si>
+    <t>nw</t>
+  </si>
+  <si>
+    <t>nf</t>
+  </si>
+  <si>
+    <t>rdf</t>
+  </si>
+  <si>
+    <t>ch</t>
+  </si>
+  <si>
+    <t>ref_ch</t>
+  </si>
+  <si>
+    <t>nh</t>
+  </si>
+  <si>
+    <t>nv</t>
+  </si>
+  <si>
+    <t>ih</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>ref_k</t>
+  </si>
+  <si>
+    <t>uk</t>
+  </si>
+  <si>
+    <t>netw</t>
+  </si>
+  <si>
+    <t>ar</t>
+  </si>
+  <si>
+    <t>vh</t>
+  </si>
+  <si>
+    <t>pch</t>
+  </si>
+  <si>
+    <t>pih</t>
+  </si>
+  <si>
+    <t>z</t>
+  </si>
+  <si>
+    <t>y3</t>
+  </si>
+  <si>
+    <t>y1</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>py0</t>
+  </si>
+  <si>
+    <t>py1</t>
+  </si>
+  <si>
+    <t>py3</t>
+  </si>
+  <si>
+    <t>ngdp</t>
+  </si>
+  <si>
+    <t>py</t>
+  </si>
+  <si>
+    <t>pk</t>
+  </si>
+  <si>
+    <t>puk</t>
+  </si>
+  <si>
+    <t>w</t>
+  </si>
+  <si>
+    <t>w0</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>rbl</t>
+  </si>
+  <si>
+    <t>bd</t>
+  </si>
+  <si>
+    <t>roc_py</t>
+  </si>
+  <si>
+    <t>ref_roc_py</t>
+  </si>
+  <si>
+    <t>roc_w</t>
+  </si>
+  <si>
+    <t>roc_pch</t>
+  </si>
+  <si>
+    <t>roc_ih</t>
+  </si>
+  <si>
+    <t>u</t>
+  </si>
+  <si>
+    <t>roc_k</t>
+  </si>
+  <si>
+    <t>ych</t>
+  </si>
+  <si>
+    <t>ycg</t>
+  </si>
+  <si>
+    <t>yih</t>
+  </si>
+  <si>
+    <t>mm</t>
+  </si>
+  <si>
+    <t>pmm</t>
+  </si>
+  <si>
+    <t>mxx</t>
+  </si>
+  <si>
+    <t>my</t>
+  </si>
+  <si>
+    <t>yxx</t>
+  </si>
+  <si>
+    <t>xx</t>
+  </si>
+  <si>
+    <t>pxx</t>
+  </si>
+  <si>
+    <t>nfa_to_ngdp</t>
+  </si>
+  <si>
+    <t>rnfa</t>
+  </si>
+  <si>
+    <t>nfa_to_ngdp_checksum</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>exp_e</t>
+  </si>
+  <si>
+    <t>roc_e</t>
+  </si>
+  <si>
+    <t>rg</t>
+  </si>
+  <si>
+    <t>pcg</t>
+  </si>
+  <si>
+    <t>cg</t>
+  </si>
+  <si>
+    <t>dg_to_ngdp</t>
+  </si>
+  <si>
+    <t>txl1</t>
+  </si>
+  <si>
+    <t>txl2</t>
+  </si>
+  <si>
+    <t>roc_cg</t>
+  </si>
+  <si>
+    <t>gg_a</t>
+  </si>
+  <si>
+    <t>gg_nn</t>
+  </si>
+  <si>
+    <t>shk_nr</t>
+  </si>
+  <si>
+    <t>shk_nw_to_nn</t>
+  </si>
+  <si>
+    <t>shk_nf_to_nw</t>
+  </si>
+  <si>
+    <t>shk_ar</t>
+  </si>
+  <si>
+    <t>shk_r</t>
+  </si>
+  <si>
+    <t>shk_w</t>
+  </si>
+  <si>
+    <t>shk_curr</t>
+  </si>
+  <si>
+    <t>shk_cg</t>
+  </si>
+  <si>
+    <t>shk_txl1</t>
+  </si>
+  <si>
+    <t>shk_txl2</t>
+  </si>
+  <si>
+    <t>gg_shk_a</t>
+  </si>
+  <si>
+    <t>gg_shk_nn</t>
+  </si>
+  <si>
+    <t>ss_nr</t>
+  </si>
+  <si>
+    <t>ss_nw_to_nn</t>
+  </si>
+  <si>
+    <t>ss_nf_to_nw</t>
+  </si>
+  <si>
+    <t>rho_nr</t>
+  </si>
+  <si>
+    <t>rho_nw</t>
+  </si>
+  <si>
+    <t>rho_nf</t>
+  </si>
+  <si>
+    <t>rho_ar</t>
+  </si>
+  <si>
+    <t>chi_curr</t>
+  </si>
+  <si>
+    <t>chi_ch</t>
+  </si>
+  <si>
+    <t>chi</t>
+  </si>
+  <si>
+    <t>nu_0</t>
+  </si>
+  <si>
+    <t>nu_1</t>
+  </si>
+  <si>
+    <t>xi_k</t>
+  </si>
+  <si>
+    <t>xi_ih</t>
+  </si>
+  <si>
+    <t>upsilon_0</t>
+  </si>
+  <si>
+    <t>upsilon_1</t>
+  </si>
+  <si>
+    <t>beta</t>
+  </si>
+  <si>
+    <t>beta_k</t>
+  </si>
+  <si>
+    <t>delta</t>
+  </si>
+  <si>
+    <t>gamma_n0</t>
+  </si>
+  <si>
+    <t>gamma_n</t>
+  </si>
+  <si>
+    <t>gamma_uk</t>
+  </si>
+  <si>
+    <t>gamma_z</t>
+  </si>
+  <si>
+    <t>eta</t>
+  </si>
+  <si>
+    <t>rho_w</t>
+  </si>
+  <si>
+    <t>kappa_1</t>
+  </si>
+  <si>
+    <t>kappa_2</t>
+  </si>
+  <si>
+    <t>ss_ar</t>
+  </si>
+  <si>
+    <t>ss_roc_pch</t>
+  </si>
+  <si>
+    <t>xi_py</t>
+  </si>
+  <si>
+    <t>mu_py</t>
+  </si>
+  <si>
+    <t>mu_y3</t>
+  </si>
+  <si>
+    <t>rho_r</t>
+  </si>
+  <si>
+    <t>psi_pch</t>
+  </si>
+  <si>
+    <t>zeta_py</t>
+  </si>
+  <si>
+    <t>xi_ch0</t>
+  </si>
+  <si>
+    <t>xi_ch1</t>
+  </si>
+  <si>
+    <t>xi_ch2</t>
+  </si>
+  <si>
+    <t>xi_y1</t>
+  </si>
+  <si>
+    <t>xi_y3</t>
+  </si>
+  <si>
+    <t>alpha</t>
+  </si>
+  <si>
+    <t>gamma_xx</t>
+  </si>
+  <si>
+    <t>theta</t>
+  </si>
+  <si>
+    <t>zeta_e</t>
+  </si>
+  <si>
+    <t>ss_dg_to_ngdp</t>
+  </si>
+  <si>
+    <t>ss_ncg_to_ngdp</t>
+  </si>
+  <si>
+    <t>tau_cg</t>
+  </si>
+  <si>
+    <t>tau_txl1</t>
+  </si>
+  <si>
+    <t>rho_cg</t>
+  </si>
+  <si>
+    <t>rho_txl2</t>
+  </si>
+  <si>
+    <t>rho_txl1</t>
+  </si>
+  <si>
+    <t>gg_rho_a</t>
+  </si>
+  <si>
+    <t>gg_ss_roc_a</t>
+  </si>
+  <si>
+    <t>gg_rho_nn</t>
+  </si>
+  <si>
+    <t>gg_ss_roc_nn</t>
+  </si>
+  <si>
+    <t>ttrend</t>
+  </si>
+  <si>
+    <t>SteadyLevel</t>
+  </si>
+  <si>
+    <t>SteadyChange</t>
+  </si>
+  <si>
+    <t>Form</t>
+  </si>
+  <si>
+    <t>Rate/</t>
+  </si>
+  <si>
+    <t>Diff-</t>
+  </si>
+  <si>
+    <t>Rate/</t>
+  </si>
+  <si>
+    <t>Diff-</t>
+  </si>
+  <si>
+    <t>Rate/</t>
+  </si>
+  <si>
+    <t>Diff-</t>
+  </si>
+  <si>
+    <t>Rate/</t>
+  </si>
+  <si>
+    <t>Diff-</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Total Population</t>
+  </si>
+  <si>
+    <t>Total Population Relative to Global Population Component</t>
+  </si>
+  <si>
+    <t>Working Age Population</t>
+  </si>
+  <si>
+    <t>Labor Force</t>
+  </si>
+  <si>
+    <t>Real Discount Factor</t>
+  </si>
+  <si>
+    <t>Private Consumption</t>
+  </si>
+  <si>
+    <t>Private Consumption, Point of Reference</t>
+  </si>
+  <si>
+    <t>Per-Capita Labor Supply</t>
+  </si>
+  <si>
+    <t>Variable Labor</t>
+  </si>
+  <si>
+    <t>Private Investment</t>
+  </si>
+  <si>
+    <t>Production Capital</t>
+  </si>
+  <si>
+    <t>Production Capital, Point of Reference</t>
+  </si>
+  <si>
+    <t>Production Capital Services</t>
+  </si>
+  <si>
+    <t>Household Net Worth</t>
+  </si>
+  <si>
+    <t>Domestic Technology Level</t>
+  </si>
+  <si>
+    <t>Shadow Value of Household Budget Constraing</t>
+  </si>
+  <si>
+    <t>Price of Private Consumption</t>
+  </si>
+  <si>
+    <t>Price of Private Investment</t>
+  </si>
+  <si>
+    <t>Roundabout Production</t>
+  </si>
+  <si>
+    <t>Stage T-2 Output</t>
+  </si>
+  <si>
+    <t>Stage T-1 Output</t>
+  </si>
+  <si>
+    <t>Stage T-0 Output</t>
+  </si>
+  <si>
+    <t>Price of Stage T-0 Output</t>
+  </si>
+  <si>
+    <t>Price of State T-1 Output</t>
+  </si>
+  <si>
+    <t>price of Stage T-2 Output</t>
+  </si>
+  <si>
+    <t>Nominal GDP</t>
+  </si>
+  <si>
+    <t>Price of Domestic Production</t>
+  </si>
+  <si>
+    <t>Price of Production Capital</t>
+  </si>
+  <si>
+    <t>Price of Production Capital Services</t>
+  </si>
+  <si>
+    <t>Nominal Wage Rate</t>
+  </si>
+  <si>
+    <t>Nominal Local Currency Money Market Rate</t>
+  </si>
+  <si>
+    <t>Nominal Local Currency Household Lending Rate</t>
+  </si>
+  <si>
+    <t>Bank Deposits</t>
+  </si>
+  <si>
+    <t>Price of Final Domestic Output, Rate of Change</t>
+  </si>
+  <si>
+    <t>Price of Final Domestic Output, Rate of Change, Point of Reference</t>
+  </si>
+  <si>
+    <t>Nominal Wage Rate, Rate of Change</t>
+  </si>
+  <si>
+    <t>Price of Consumer Goods, Rate of Change</t>
+  </si>
+  <si>
+    <t>Household Investment, Rate of Change</t>
+  </si>
+  <si>
+    <t>Capital Utilization Rate</t>
+  </si>
+  <si>
+    <t>Household Capital, Rate of Change</t>
+  </si>
+  <si>
+    <t>Domestic Component of Private Consumption</t>
+  </si>
+  <si>
+    <t>Domestic Component of Government Consumption</t>
+  </si>
+  <si>
+    <t>Domestic Component of Private Investment</t>
+  </si>
+  <si>
+    <t>Total Non-Commodity Imports</t>
+  </si>
+  <si>
+    <t>Price of Imports</t>
+  </si>
+  <si>
+    <t>Import Content of Non-Commodity Exports</t>
+  </si>
+  <si>
+    <t>Intermediate Import Inputs into Domestic Production</t>
+  </si>
+  <si>
+    <t>Domestic Content of Non-Commodity Exports</t>
+  </si>
+  <si>
+    <t>Non-Commodity Exports</t>
+  </si>
+  <si>
+    <t>Price of Non-Commodity Exports</t>
+  </si>
+  <si>
+    <t>Net Foreign Assets to GDP Ratio</t>
+  </si>
+  <si>
+    <t>Effective Interest Rate and Valuation on NFA</t>
+  </si>
+  <si>
+    <t>Checksum for Net Foreign Assets to GDP Ratio</t>
+  </si>
+  <si>
+    <t>Nominal Exchange Rate</t>
+  </si>
+  <si>
+    <t>Expectations of Nominal Exchange Rate</t>
+  </si>
+  <si>
+    <t>Nominal Exchange Rate, Rate of Change</t>
+  </si>
+  <si>
+    <t>Government Debt Interest Rate</t>
+  </si>
+  <si>
+    <t>Price of Government Consumption</t>
+  </si>
+  <si>
+    <t>Government Consumption</t>
+  </si>
+  <si>
+    <t>Government Debt to GDP Ratio</t>
+  </si>
+  <si>
+    <t>Net Lump-Sum Tax Rate on Wealthy Consumers</t>
+  </si>
+  <si>
+    <t>Net Lump-Sum Tax Rate on Poor Consumers</t>
+  </si>
+  <si>
+    <t>Government Consumption, Rate of Change</t>
+  </si>
+  <si>
+    <t>S/S Population, Relative to Global Population Component</t>
+  </si>
+  <si>
+    <t>S/S Share of Working Age Population in Total Population</t>
+  </si>
+  <si>
+    <t>S/S Labor Participation Rate</t>
+  </si>
+  <si>
+    <t>Autoregression in Total Population Relative to Global Population Component</t>
+  </si>
+  <si>
+    <t>Autoregression in Share of Working Age Population in Total Population</t>
+  </si>
+  <si>
+    <t>Autoregression in Labor Participation Rate</t>
+  </si>
+  <si>
+    <t>Import Intensity of Non-Commodity Exports</t>
+  </si>
+  <si>
+    <t>Acceleration in Exportable Productivity</t>
+  </si>
+  <si>
+    <t>Elasticity of Household Lending Rate to Risk</t>
+  </si>
+  <si>
+    <t>Weight on Model-Consistent Expectations in Exchange Rate</t>
+  </si>
+  <si>
+    <t>Time trend</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>nn</t>
+  </si>
+  <si>
+    <t>nr</t>
+  </si>
+  <si>
+    <t>nw</t>
+  </si>
+  <si>
+    <t>nf</t>
+  </si>
+  <si>
+    <t>rdf</t>
+  </si>
+  <si>
+    <t>ch</t>
+  </si>
+  <si>
+    <t>ref_ch</t>
+  </si>
+  <si>
+    <t>nh</t>
+  </si>
+  <si>
+    <t>nv</t>
+  </si>
+  <si>
+    <t>ih</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>ref_k</t>
+  </si>
+  <si>
+    <t>uk</t>
+  </si>
+  <si>
+    <t>netw</t>
+  </si>
+  <si>
+    <t>ar</t>
+  </si>
+  <si>
+    <t>vh</t>
+  </si>
+  <si>
+    <t>pch</t>
+  </si>
+  <si>
+    <t>pih</t>
+  </si>
+  <si>
+    <t>z</t>
+  </si>
+  <si>
+    <t>y3</t>
+  </si>
+  <si>
+    <t>y1</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>py0</t>
+  </si>
+  <si>
+    <t>py1</t>
+  </si>
+  <si>
+    <t>py3</t>
+  </si>
+  <si>
+    <t>ngdp</t>
+  </si>
+  <si>
+    <t>py</t>
+  </si>
+  <si>
+    <t>pk</t>
+  </si>
+  <si>
+    <t>puk</t>
+  </si>
+  <si>
+    <t>w</t>
+  </si>
+  <si>
+    <t>w0</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>rbl</t>
+  </si>
+  <si>
+    <t>bd</t>
+  </si>
+  <si>
+    <t>roc_py</t>
+  </si>
+  <si>
+    <t>ref_roc_py</t>
+  </si>
+  <si>
+    <t>roc_w</t>
+  </si>
+  <si>
+    <t>roc_pch</t>
+  </si>
+  <si>
+    <t>roc_ih</t>
+  </si>
+  <si>
+    <t>u</t>
+  </si>
+  <si>
+    <t>roc_k</t>
+  </si>
+  <si>
+    <t>ych</t>
+  </si>
+  <si>
+    <t>ycg</t>
+  </si>
+  <si>
+    <t>yih</t>
+  </si>
+  <si>
+    <t>mm</t>
+  </si>
+  <si>
+    <t>pmm</t>
+  </si>
+  <si>
+    <t>mxx</t>
+  </si>
+  <si>
+    <t>my</t>
+  </si>
+  <si>
+    <t>yxx</t>
+  </si>
+  <si>
+    <t>xx</t>
+  </si>
+  <si>
+    <t>pxx</t>
+  </si>
+  <si>
+    <t>nfa_to_ngdp</t>
+  </si>
+  <si>
+    <t>rnfa</t>
+  </si>
+  <si>
+    <t>nfa_to_ngdp_checksum</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>exp_e</t>
+  </si>
+  <si>
+    <t>roc_e</t>
+  </si>
+  <si>
+    <t>rg</t>
+  </si>
+  <si>
+    <t>pcg</t>
+  </si>
+  <si>
+    <t>cg</t>
+  </si>
+  <si>
+    <t>dg_to_ngdp</t>
+  </si>
+  <si>
+    <t>txl1</t>
+  </si>
+  <si>
+    <t>txl2</t>
+  </si>
+  <si>
+    <t>roc_cg</t>
+  </si>
+  <si>
+    <t>gg_a</t>
+  </si>
+  <si>
+    <t>gg_nn</t>
+  </si>
+  <si>
+    <t>shk_nr</t>
+  </si>
+  <si>
+    <t>shk_nw_to_nn</t>
+  </si>
+  <si>
+    <t>shk_nf_to_nw</t>
+  </si>
+  <si>
+    <t>shk_ar</t>
+  </si>
+  <si>
+    <t>shk_r</t>
+  </si>
+  <si>
+    <t>shk_w</t>
+  </si>
+  <si>
+    <t>shk_curr</t>
+  </si>
+  <si>
+    <t>shk_cg</t>
+  </si>
+  <si>
+    <t>shk_txl1</t>
+  </si>
+  <si>
+    <t>shk_txl2</t>
+  </si>
+  <si>
+    <t>gg_shk_a</t>
+  </si>
+  <si>
+    <t>gg_shk_nn</t>
+  </si>
+  <si>
+    <t>ss_nr</t>
+  </si>
+  <si>
+    <t>ss_nw_to_nn</t>
+  </si>
+  <si>
+    <t>ss_nf_to_nw</t>
+  </si>
+  <si>
+    <t>rho_nr</t>
+  </si>
+  <si>
+    <t>rho_nw</t>
+  </si>
+  <si>
+    <t>rho_nf</t>
+  </si>
+  <si>
+    <t>rho_ar</t>
+  </si>
+  <si>
+    <t>chi_curr</t>
+  </si>
+  <si>
+    <t>chi_ch</t>
+  </si>
+  <si>
+    <t>chi</t>
+  </si>
+  <si>
+    <t>nu_0</t>
+  </si>
+  <si>
+    <t>nu_1</t>
+  </si>
+  <si>
+    <t>xi_k</t>
+  </si>
+  <si>
+    <t>xi_ih</t>
+  </si>
+  <si>
+    <t>upsilon_0</t>
+  </si>
+  <si>
+    <t>upsilon_1</t>
+  </si>
+  <si>
+    <t>beta</t>
+  </si>
+  <si>
+    <t>beta_k</t>
+  </si>
+  <si>
+    <t>delta</t>
+  </si>
+  <si>
+    <t>gamma_n0</t>
+  </si>
+  <si>
+    <t>gamma_n</t>
+  </si>
+  <si>
+    <t>gamma_uk</t>
+  </si>
+  <si>
+    <t>gamma_z</t>
+  </si>
+  <si>
+    <t>eta</t>
+  </si>
+  <si>
+    <t>rho_w</t>
+  </si>
+  <si>
+    <t>kappa_1</t>
+  </si>
+  <si>
+    <t>kappa_2</t>
+  </si>
+  <si>
+    <t>ss_ar</t>
+  </si>
+  <si>
+    <t>ss_roc_pch</t>
+  </si>
+  <si>
+    <t>xi_py</t>
+  </si>
+  <si>
+    <t>mu_py</t>
+  </si>
+  <si>
+    <t>mu_y3</t>
+  </si>
+  <si>
+    <t>rho_r</t>
+  </si>
+  <si>
+    <t>psi_pch</t>
+  </si>
+  <si>
+    <t>zeta_py</t>
+  </si>
+  <si>
+    <t>xi_ch0</t>
+  </si>
+  <si>
+    <t>xi_ch1</t>
+  </si>
+  <si>
+    <t>xi_ch2</t>
+  </si>
+  <si>
+    <t>xi_y1</t>
+  </si>
+  <si>
+    <t>xi_y3</t>
   </si>
   <si>
     <t>alpha</t>
@@ -2688,7 +4677,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -2700,16 +4689,22 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2731,24 +4726,24 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>664</v>
+        <v>1327</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>799</v>
+        <v>1462</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>800</v>
+        <v>1463</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>801</v>
+        <v>1464</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>810</v>
+        <v>1473</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>665</v>
+        <v>1328</v>
       </c>
       <c r="B2" s="0">
         <v>1</v>
@@ -2757,15 +4752,15 @@
         <v>1</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>802</v>
+        <v>1465</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>811</v>
+        <v>1474</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>666</v>
+        <v>1329</v>
       </c>
       <c r="B3" s="0">
         <v>1</v>
@@ -2774,15 +4769,15 @@
         <v>1</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>802</v>
+        <v>1465</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>812</v>
+        <v>1475</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>667</v>
+        <v>1330</v>
       </c>
       <c r="B4" s="0">
         <v>0.69999999999999996</v>
@@ -2791,15 +4786,15 @@
         <v>1</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>802</v>
+        <v>1465</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>813</v>
+        <v>1476</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>668</v>
+        <v>1331</v>
       </c>
       <c r="B5" s="0">
         <v>0.48999999999999994</v>
@@ -2808,185 +4803,185 @@
         <v>1</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>802</v>
+        <v>1465</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>814</v>
+        <v>1477</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="s">
-        <v>669</v>
+        <v>1332</v>
       </c>
       <c r="B6" s="0">
-        <v>0.95000000000000018</v>
+        <v>0.94999999999999973</v>
       </c>
       <c r="C6" s="0">
         <v>1</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>802</v>
+        <v>1465</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>815</v>
+        <v>1478</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0" t="s">
-        <v>670</v>
+        <v>1333</v>
       </c>
       <c r="B7" s="0">
-        <v>0.50008269044960352</v>
+        <v>0.50008269044960318</v>
       </c>
       <c r="C7" s="0">
-        <v>0.99999999999999989</v>
+        <v>1.0000000000000002</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>802</v>
+        <v>1465</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>816</v>
+        <v>1479</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0" t="s">
-        <v>671</v>
+        <v>1334</v>
       </c>
       <c r="B8" s="0">
-        <v>0.078399999999999984</v>
+        <v>0.097999999999999976</v>
       </c>
       <c r="C8" s="0">
-        <v>0.99999999999999978</v>
+        <v>1.0000000000000002</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>802</v>
+        <v>1465</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>817</v>
+        <v>1480</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0" t="s">
-        <v>672</v>
+        <v>1335</v>
       </c>
       <c r="B9" s="0">
-        <v>1.5997354343153787</v>
+        <v>1.9996692928942255</v>
       </c>
       <c r="C9" s="0">
-        <v>0.99999999999999989</v>
+        <v>1</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>802</v>
+        <v>1465</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>818</v>
+        <v>1481</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0" t="s">
-        <v>673</v>
+        <v>1336</v>
       </c>
       <c r="B10" s="0">
-        <v>0.78387036281453559</v>
+        <v>0.65322530234544696</v>
       </c>
       <c r="C10" s="0">
         <v>1</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>802</v>
+        <v>1465</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>819</v>
+        <v>1482</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0" t="s">
-        <v>674</v>
+        <v>1337</v>
       </c>
       <c r="B11" s="0">
-        <v>0.13191730955039646</v>
+        <v>0.13191730955039685</v>
       </c>
       <c r="C11" s="0">
-        <v>1</v>
+        <v>1.0000000000000002</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>802</v>
+        <v>1465</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>820</v>
+        <v>1483</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0" t="s">
-        <v>675</v>
+        <v>1338</v>
       </c>
       <c r="B12" s="0">
-        <v>0.87944873033597792</v>
+        <v>0.87944873033597726</v>
       </c>
       <c r="C12" s="0">
-        <v>0.99999999999999989</v>
+        <v>1.0000000000000002</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>802</v>
+        <v>1465</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>821</v>
+        <v>1484</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0" t="s">
-        <v>676</v>
+        <v>1339</v>
       </c>
       <c r="B13" s="0">
-        <v>0.87944873033597804</v>
+        <v>0.87944873033597726</v>
       </c>
       <c r="C13" s="0">
-        <v>0.99999999999999978</v>
+        <v>1.0000000000000002</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>802</v>
+        <v>1465</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>822</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0" t="s">
-        <v>677</v>
+        <v>1340</v>
       </c>
       <c r="B14" s="0">
-        <v>0.87944873033597792</v>
+        <v>0.87944873033597726</v>
       </c>
       <c r="C14" s="0">
-        <v>0.99999999999999989</v>
+        <v>1.0000000000000002</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>802</v>
+        <v>1465</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>823</v>
+        <v>1486</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0" t="s">
-        <v>678</v>
+        <v>1341</v>
       </c>
       <c r="B15" s="0">
-        <v>0.023447598398196167</v>
+        <v>0.023447598398196177</v>
       </c>
       <c r="C15" s="0">
-        <v>1</v>
+        <v>0.99999999999999978</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>802</v>
+        <v>1465</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>824</v>
+        <v>1487</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0" t="s">
-        <v>679</v>
+        <v>1342</v>
       </c>
       <c r="B16" s="0">
         <v>1</v>
@@ -2995,32 +4990,32 @@
         <v>1</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>802</v>
+        <v>1465</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>825</v>
+        <v>1488</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0" t="s">
-        <v>680</v>
+        <v>1343</v>
       </c>
       <c r="B17" s="0">
-        <v>1.9996692928942241</v>
+        <v>1.9996692928942259</v>
       </c>
       <c r="C17" s="0">
-        <v>1.0000000000000002</v>
+        <v>0.99999999999999978</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>802</v>
+        <v>1465</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>826</v>
+        <v>1489</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0" t="s">
-        <v>681</v>
+        <v>1344</v>
       </c>
       <c r="B18" s="0">
         <v>1</v>
@@ -3029,15 +5024,15 @@
         <v>1</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>802</v>
+        <v>1465</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>827</v>
+        <v>1490</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0" t="s">
-        <v>682</v>
+        <v>1345</v>
       </c>
       <c r="B19" s="0">
         <v>1</v>
@@ -3046,83 +5041,83 @@
         <v>1</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>802</v>
+        <v>1465</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>828</v>
+        <v>1491</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0" t="s">
-        <v>683</v>
+        <v>1346</v>
       </c>
       <c r="B20" s="0">
-        <v>1.1999999999999995</v>
+        <v>1.2</v>
       </c>
       <c r="C20" s="0">
-        <v>0.99999999999999978</v>
+        <v>1.0000000000000002</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>802</v>
+        <v>1465</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>829</v>
+        <v>1492</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0" t="s">
-        <v>684</v>
+        <v>1347</v>
       </c>
       <c r="B21" s="0">
-        <v>3.259005045157648</v>
+        <v>3.2590050451576511</v>
       </c>
       <c r="C21" s="0">
-        <v>0.99999999999999989</v>
+        <v>1</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>802</v>
+        <v>1465</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>830</v>
+        <v>1493</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0" t="s">
-        <v>685</v>
+        <v>1348</v>
       </c>
       <c r="B22" s="0">
-        <v>2.1999999999999993</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="C22" s="0">
-        <v>0.99999999999999989</v>
+        <v>1</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>802</v>
+        <v>1465</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>831</v>
+        <v>1494</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0" t="s">
-        <v>686</v>
+        <v>1349</v>
       </c>
       <c r="B23" s="0">
         <v>1</v>
       </c>
       <c r="C23" s="0">
-        <v>0.99999999999999978</v>
+        <v>1.0000000000000002</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>802</v>
+        <v>1465</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>832</v>
+        <v>1495</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0" t="s">
-        <v>687</v>
+        <v>1350</v>
       </c>
       <c r="B24" s="0">
         <v>0.90909090909090906</v>
@@ -3131,15 +5126,15 @@
         <v>1</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>802</v>
+        <v>1465</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>833</v>
+        <v>1496</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0" t="s">
-        <v>688</v>
+        <v>1351</v>
       </c>
       <c r="B25" s="0">
         <v>0.36363636363636365</v>
@@ -3148,49 +5143,49 @@
         <v>1</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>802</v>
+        <v>1465</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>834</v>
+        <v>1497</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0" t="s">
-        <v>689</v>
+        <v>1352</v>
       </c>
       <c r="B26" s="0">
-        <v>0.17183158425362635</v>
+        <v>0.17183158425362627</v>
       </c>
       <c r="C26" s="0">
         <v>1</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>802</v>
+        <v>1465</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>835</v>
+        <v>1498</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0" t="s">
-        <v>690</v>
+        <v>1353</v>
       </c>
       <c r="B27" s="0">
         <v>1</v>
       </c>
       <c r="C27" s="0">
-        <v>0.99999999999999978</v>
+        <v>1.0000000000000002</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>802</v>
+        <v>1465</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>836</v>
+        <v>1499</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0" t="s">
-        <v>691</v>
+        <v>1354</v>
       </c>
       <c r="B28" s="0">
         <v>1</v>
@@ -3199,15 +5194,15 @@
         <v>1</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>802</v>
+        <v>1465</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>837</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0" t="s">
-        <v>692</v>
+        <v>1355</v>
       </c>
       <c r="B29" s="0">
         <v>1</v>
@@ -3216,115 +5211,115 @@
         <v>1</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>802</v>
+        <v>1465</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>838</v>
+        <v>1501</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0" t="s">
-        <v>693</v>
+        <v>1356</v>
       </c>
       <c r="B30" s="0">
-        <v>0.27289822785725343</v>
+        <v>0.27289822785725365</v>
       </c>
       <c r="C30" s="0">
-        <v>1</v>
+        <v>0.99999999999999989</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>802</v>
+        <v>1465</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>839</v>
+        <v>1502</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0" t="s">
-        <v>694</v>
+        <v>1357</v>
       </c>
       <c r="B31" s="0">
-        <v>0.50008269044960363</v>
+        <v>0.50008269044960318</v>
       </c>
       <c r="C31" s="0">
-        <v>0.99999999999999989</v>
+        <v>1.0000000000000002</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>802</v>
+        <v>1465</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>840</v>
+        <v>1503</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0" t="s">
-        <v>695</v>
+        <v>1358</v>
       </c>
       <c r="B32" s="0">
-        <v>0.50008269044960352</v>
+        <v>0.50008269044960318</v>
       </c>
       <c r="C32" s="0">
-        <v>0.99999999999999989</v>
+        <v>1.0000000000000002</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>802</v>
+        <v>1465</v>
       </c>
       <c r="E32" s="0"/>
     </row>
     <row r="33">
       <c r="A33" s="0" t="s">
-        <v>696</v>
+        <v>1359</v>
       </c>
       <c r="B33" s="0">
-        <v>1.0522612924813191</v>
+        <v>1.0522612924813197</v>
       </c>
       <c r="C33" s="0">
         <v>1</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>802</v>
+        <v>1465</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>841</v>
+        <v>1504</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0" t="s">
-        <v>697</v>
+        <v>1360</v>
       </c>
       <c r="B34" s="0">
-        <v>1.0522612924813193</v>
+        <v>1.0522612924813197</v>
       </c>
       <c r="C34" s="0">
         <v>1</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>802</v>
+        <v>1465</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>842</v>
+        <v>1505</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0" t="s">
-        <v>698</v>
+        <v>1361</v>
       </c>
       <c r="B35" s="0">
-        <v>0.35997243651679894</v>
+        <v>0.35997243651679889</v>
       </c>
       <c r="C35" s="0">
-        <v>0.99999999999999978</v>
+        <v>1.0000000000000002</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>802</v>
+        <v>1465</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>843</v>
+        <v>1506</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0" t="s">
-        <v>699</v>
+        <v>1362</v>
       </c>
       <c r="B36" s="0">
         <v>1</v>
@@ -3333,15 +5328,15 @@
         <v>1</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>802</v>
+        <v>1465</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>844</v>
+        <v>1507</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0" t="s">
-        <v>700</v>
+        <v>1363</v>
       </c>
       <c r="B37" s="0">
         <v>1</v>
@@ -3350,32 +5345,32 @@
         <v>1</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>802</v>
+        <v>1465</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>845</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0" t="s">
-        <v>701</v>
+        <v>1364</v>
       </c>
       <c r="B38" s="0">
-        <v>0.99999999999999989</v>
+        <v>1.0000000000000002</v>
       </c>
       <c r="C38" s="0">
         <v>1</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>802</v>
+        <v>1465</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>846</v>
+        <v>1509</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0" t="s">
-        <v>702</v>
+        <v>1365</v>
       </c>
       <c r="B39" s="0">
         <v>1</v>
@@ -3384,32 +5379,32 @@
         <v>1</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>802</v>
+        <v>1465</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>847</v>
+        <v>1510</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0" t="s">
-        <v>703</v>
+        <v>1366</v>
       </c>
       <c r="B40" s="0">
-        <v>0.99999999999999989</v>
+        <v>1.0000000000000002</v>
       </c>
       <c r="C40" s="0">
         <v>1</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>802</v>
+        <v>1465</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>848</v>
+        <v>1511</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0" t="s">
-        <v>704</v>
+        <v>1367</v>
       </c>
       <c r="B41" s="0">
         <v>1</v>
@@ -3418,253 +5413,253 @@
         <v>1</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>802</v>
+        <v>1465</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>849</v>
+        <v>1512</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0" t="s">
-        <v>705</v>
+        <v>1368</v>
       </c>
       <c r="B42" s="0">
-        <v>0.99999999999999978</v>
+        <v>1.0000000000000002</v>
       </c>
       <c r="C42" s="0">
-        <v>1.0000000000000002</v>
+        <v>1</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>802</v>
+        <v>1465</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>850</v>
+        <v>1513</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0" t="s">
-        <v>706</v>
+        <v>1369</v>
       </c>
       <c r="B43" s="0">
-        <v>0.50008269044960352</v>
+        <v>0.50008269044960318</v>
       </c>
       <c r="C43" s="0">
-        <v>0.99999999999999989</v>
+        <v>1.0000000000000002</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>802</v>
+        <v>1465</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>851</v>
+        <v>1514</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0" t="s">
-        <v>707</v>
+        <v>1370</v>
       </c>
       <c r="B44" s="0">
         <v>0.20000000000000001</v>
       </c>
       <c r="C44" s="0">
-        <v>0.99999999999999978</v>
+        <v>1.0000000000000002</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>802</v>
+        <v>1465</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>852</v>
+        <v>1515</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="0" t="s">
-        <v>708</v>
+        <v>1371</v>
       </c>
       <c r="B45" s="0">
-        <v>0.13191730955039646</v>
+        <v>0.13191730955039685</v>
       </c>
       <c r="C45" s="0">
-        <v>1</v>
+        <v>1.0000000000000002</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>802</v>
+        <v>1465</v>
       </c>
       <c r="E45" s="0" t="s">
-        <v>853</v>
+        <v>1516</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="0" t="s">
-        <v>709</v>
+        <v>1372</v>
       </c>
       <c r="B46" s="0">
-        <v>0.083999999999999964</v>
+        <v>0.33599999999999997</v>
       </c>
       <c r="C46" s="0">
-        <v>0.99999999999999989</v>
+        <v>1.0000000000000002</v>
       </c>
       <c r="D46" s="0" t="s">
-        <v>802</v>
+        <v>1465</v>
       </c>
       <c r="E46" s="0" t="s">
-        <v>854</v>
+        <v>1517</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="0" t="s">
-        <v>710</v>
+        <v>1373</v>
       </c>
       <c r="B47" s="0">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C47" s="0">
         <v>1</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>802</v>
+        <v>1465</v>
       </c>
       <c r="E47" s="0" t="s">
-        <v>855</v>
+        <v>1518</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="0" t="s">
-        <v>711</v>
+        <v>1374</v>
       </c>
       <c r="B48" s="0">
-        <v>0.041999999999999975</v>
+        <v>0.16800000000000001</v>
       </c>
       <c r="C48" s="0">
-        <v>0.99999999999999978</v>
+        <v>1.0000000000000002</v>
       </c>
       <c r="D48" s="0" t="s">
-        <v>802</v>
+        <v>1465</v>
       </c>
       <c r="E48" s="0" t="s">
-        <v>856</v>
+        <v>1519</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="0" t="s">
-        <v>712</v>
+        <v>1375</v>
       </c>
       <c r="B49" s="0">
-        <v>0.041999999999999975</v>
+        <v>0.16800000000000001</v>
       </c>
       <c r="C49" s="0">
-        <v>0.99999999999999978</v>
+        <v>1.0000000000000002</v>
       </c>
       <c r="D49" s="0" t="s">
-        <v>802</v>
+        <v>1465</v>
       </c>
       <c r="E49" s="0" t="s">
-        <v>857</v>
+        <v>1520</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="0" t="s">
-        <v>713</v>
+        <v>1376</v>
       </c>
       <c r="B50" s="0">
-        <v>0.16799999999999993</v>
+        <v>0.16799999999999998</v>
       </c>
       <c r="C50" s="0">
-        <v>0.99999999999999989</v>
+        <v>1.0000000000000002</v>
       </c>
       <c r="D50" s="0" t="s">
-        <v>802</v>
+        <v>1465</v>
       </c>
       <c r="E50" s="0" t="s">
-        <v>858</v>
+        <v>1521</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="0" t="s">
-        <v>714</v>
+        <v>1377</v>
       </c>
       <c r="B51" s="0">
-        <v>0.083999999999999964</v>
+        <v>0.33599999999999997</v>
       </c>
       <c r="C51" s="0">
-        <v>0.99999999999999978</v>
+        <v>1.0000000000000002</v>
       </c>
       <c r="D51" s="0" t="s">
-        <v>802</v>
+        <v>1465</v>
       </c>
       <c r="E51" s="0" t="s">
-        <v>859</v>
+        <v>1522</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="0" t="s">
-        <v>715</v>
+        <v>1378</v>
       </c>
       <c r="B52" s="0">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C52" s="0">
         <v>1</v>
       </c>
       <c r="D52" s="0" t="s">
-        <v>802</v>
+        <v>1465</v>
       </c>
       <c r="E52" s="0" t="s">
-        <v>860</v>
+        <v>1523</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="0" t="s">
-        <v>716</v>
+        <v>1379</v>
       </c>
       <c r="B53" s="0">
-        <v>1.8765109733383411e-20</v>
+        <v>-1.6099935554079168e-23</v>
       </c>
       <c r="C53" s="0">
-        <v>-1.0543252698567548e-20</v>
+        <v>4.9702343377700478e-24</v>
       </c>
       <c r="D53" s="0" t="s">
-        <v>803</v>
+        <v>1466</v>
       </c>
       <c r="E53" s="0" t="s">
-        <v>861</v>
+        <v>1524</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="0" t="s">
-        <v>717</v>
+        <v>1380</v>
       </c>
       <c r="B54" s="0">
-        <v>1.0522612924813193</v>
+        <v>1.0522612924813197</v>
       </c>
       <c r="C54" s="0">
         <v>1</v>
       </c>
       <c r="D54" s="0" t="s">
-        <v>804</v>
+        <v>1467</v>
       </c>
       <c r="E54" s="0" t="s">
-        <v>862</v>
+        <v>1525</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="0" t="s">
-        <v>718</v>
+        <v>1381</v>
       </c>
       <c r="B55" s="0">
         <v>0</v>
       </c>
       <c r="C55" s="0">
-        <v>-8.0346333522937322e-23</v>
+        <v>-2.0170224257040672e-24</v>
       </c>
       <c r="D55" s="0" t="s">
-        <v>805</v>
+        <v>1468</v>
       </c>
       <c r="E55" s="0" t="s">
-        <v>863</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="0" t="s">
-        <v>719</v>
+        <v>1382</v>
       </c>
       <c r="B56" s="0">
         <v>1</v>
@@ -3673,15 +5668,15 @@
         <v>1</v>
       </c>
       <c r="D56" s="0" t="s">
-        <v>806</v>
+        <v>1469</v>
       </c>
       <c r="E56" s="0" t="s">
-        <v>864</v>
+        <v>1527</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="0" t="s">
-        <v>720</v>
+        <v>1383</v>
       </c>
       <c r="B57" s="0">
         <v>1</v>
@@ -3690,15 +5685,15 @@
         <v>1</v>
       </c>
       <c r="D57" s="0" t="s">
-        <v>806</v>
+        <v>1469</v>
       </c>
       <c r="E57" s="0" t="s">
-        <v>865</v>
+        <v>1528</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="0" t="s">
-        <v>721</v>
+        <v>1384</v>
       </c>
       <c r="B58" s="0">
         <v>1</v>
@@ -3707,32 +5702,32 @@
         <v>1</v>
       </c>
       <c r="D58" s="0" t="s">
-        <v>806</v>
+        <v>1469</v>
       </c>
       <c r="E58" s="0" t="s">
-        <v>866</v>
+        <v>1529</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="0" t="s">
-        <v>722</v>
+        <v>1385</v>
       </c>
       <c r="B59" s="0">
-        <v>1.0522612924813193</v>
+        <v>1.0522612924813197</v>
       </c>
       <c r="C59" s="0">
         <v>1</v>
       </c>
       <c r="D59" s="0" t="s">
-        <v>806</v>
+        <v>1469</v>
       </c>
       <c r="E59" s="0" t="s">
-        <v>867</v>
+        <v>1530</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="0" t="s">
-        <v>723</v>
+        <v>1386</v>
       </c>
       <c r="B60" s="0">
         <v>1</v>
@@ -3741,115 +5736,115 @@
         <v>1</v>
       </c>
       <c r="D60" s="0" t="s">
-        <v>806</v>
+        <v>1469</v>
       </c>
       <c r="E60" s="0" t="s">
-        <v>868</v>
+        <v>1531</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="0" t="s">
-        <v>724</v>
+        <v>1387</v>
       </c>
       <c r="B61" s="0">
         <v>0.20000000000000001</v>
       </c>
       <c r="C61" s="0">
-        <v>0.99999999999999978</v>
+        <v>1.0000000000000002</v>
       </c>
       <c r="D61" s="0" t="s">
-        <v>806</v>
+        <v>1469</v>
       </c>
       <c r="E61" s="0" t="s">
-        <v>869</v>
+        <v>1532</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="0" t="s">
-        <v>725</v>
+        <v>1388</v>
       </c>
       <c r="B62" s="0">
         <v>0.40000000000000002</v>
       </c>
       <c r="C62" s="0">
-        <v>-2.674226936507312e-18</v>
+        <v>-5.5201881558760866e-18</v>
       </c>
       <c r="D62" s="0" t="s">
-        <v>807</v>
+        <v>1470</v>
       </c>
       <c r="E62" s="0" t="s">
-        <v>870</v>
+        <v>1533</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="0" t="s">
-        <v>726</v>
+        <v>1389</v>
       </c>
       <c r="B63" s="0">
-        <v>0.44173597929158825</v>
+        <v>0.44173597929158853</v>
       </c>
       <c r="C63" s="0">
-        <v>1.2951876477472776e-17</v>
+        <v>3.187624680146671e-17</v>
       </c>
       <c r="D63" s="0" t="s">
-        <v>807</v>
+        <v>1470</v>
       </c>
       <c r="E63" s="0" t="s">
-        <v>871</v>
+        <v>1534</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="0" t="s">
-        <v>727</v>
+        <v>1390</v>
       </c>
       <c r="B64" s="0">
-        <v>-3.2730325458321706e-23</v>
+        <v>-1.7222970750961509e-27</v>
       </c>
       <c r="C64" s="0">
-        <v>1.0901882904653486e-23</v>
+        <v>5.8085780746951304e-28</v>
       </c>
       <c r="D64" s="0" t="s">
-        <v>807</v>
+        <v>1470</v>
       </c>
       <c r="E64" s="0" t="s">
-        <v>872</v>
+        <v>1535</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="0" t="s">
-        <v>728</v>
+        <v>1391</v>
       </c>
       <c r="B65" s="0">
-        <v>0.99999999999999978</v>
+        <v>1.0000000000000002</v>
       </c>
       <c r="C65" s="0">
         <v>1</v>
       </c>
       <c r="D65" s="0" t="s">
-        <v>808</v>
+        <v>1471</v>
       </c>
       <c r="E65" s="0" t="s">
-        <v>873</v>
+        <v>1536</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="0" t="s">
-        <v>729</v>
+        <v>1392</v>
       </c>
       <c r="B66" s="0">
-        <v>26.839251011899048</v>
+        <v>17.779761358258192</v>
       </c>
       <c r="C66" s="0">
         <v>1</v>
       </c>
       <c r="D66" s="0" t="s">
-        <v>808</v>
+        <v>1471</v>
       </c>
       <c r="E66" s="0"/>
     </row>
     <row r="67">
       <c r="A67" s="0" t="s">
-        <v>730</v>
+        <v>1393</v>
       </c>
       <c r="B67" s="0">
         <v>1</v>
@@ -3858,13 +5853,13 @@
         <v>1</v>
       </c>
       <c r="D67" s="0" t="s">
-        <v>808</v>
+        <v>1471</v>
       </c>
       <c r="E67" s="0"/>
     </row>
     <row r="68">
       <c r="A68" s="0" t="s">
-        <v>731</v>
+        <v>1394</v>
       </c>
       <c r="B68" s="0">
         <v>0</v>
@@ -3873,13 +5868,13 @@
         <v>0</v>
       </c>
       <c r="D68" s="0" t="s">
-        <v>809</v>
+        <v>1472</v>
       </c>
       <c r="E68" s="0"/>
     </row>
     <row r="69">
       <c r="A69" s="0" t="s">
-        <v>732</v>
+        <v>1395</v>
       </c>
       <c r="B69" s="0">
         <v>0</v>
@@ -3888,13 +5883,13 @@
         <v>0</v>
       </c>
       <c r="D69" s="0" t="s">
-        <v>809</v>
+        <v>1472</v>
       </c>
       <c r="E69" s="0"/>
     </row>
     <row r="70">
       <c r="A70" s="0" t="s">
-        <v>733</v>
+        <v>1396</v>
       </c>
       <c r="B70" s="0">
         <v>0</v>
@@ -3903,13 +5898,13 @@
         <v>0</v>
       </c>
       <c r="D70" s="0" t="s">
-        <v>809</v>
+        <v>1472</v>
       </c>
       <c r="E70" s="0"/>
     </row>
     <row r="71">
       <c r="A71" s="0" t="s">
-        <v>734</v>
+        <v>1397</v>
       </c>
       <c r="B71" s="0">
         <v>0</v>
@@ -3918,13 +5913,13 @@
         <v>0</v>
       </c>
       <c r="D71" s="0" t="s">
-        <v>809</v>
+        <v>1472</v>
       </c>
       <c r="E71" s="0"/>
     </row>
     <row r="72">
       <c r="A72" s="0" t="s">
-        <v>735</v>
+        <v>1398</v>
       </c>
       <c r="B72" s="0">
         <v>0</v>
@@ -3933,13 +5928,13 @@
         <v>0</v>
       </c>
       <c r="D72" s="0" t="s">
-        <v>809</v>
+        <v>1472</v>
       </c>
       <c r="E72" s="0"/>
     </row>
     <row r="73">
       <c r="A73" s="0" t="s">
-        <v>736</v>
+        <v>1399</v>
       </c>
       <c r="B73" s="0">
         <v>0</v>
@@ -3948,13 +5943,13 @@
         <v>0</v>
       </c>
       <c r="D73" s="0" t="s">
-        <v>809</v>
+        <v>1472</v>
       </c>
       <c r="E73" s="0"/>
     </row>
     <row r="74">
       <c r="A74" s="0" t="s">
-        <v>737</v>
+        <v>1400</v>
       </c>
       <c r="B74" s="0">
         <v>0</v>
@@ -3963,13 +5958,13 @@
         <v>0</v>
       </c>
       <c r="D74" s="0" t="s">
-        <v>809</v>
+        <v>1472</v>
       </c>
       <c r="E74" s="0"/>
     </row>
     <row r="75">
       <c r="A75" s="0" t="s">
-        <v>738</v>
+        <v>1401</v>
       </c>
       <c r="B75" s="0">
         <v>0</v>
@@ -3978,13 +5973,13 @@
         <v>0</v>
       </c>
       <c r="D75" s="0" t="s">
-        <v>809</v>
+        <v>1472</v>
       </c>
       <c r="E75" s="0"/>
     </row>
     <row r="76">
       <c r="A76" s="0" t="s">
-        <v>739</v>
+        <v>1402</v>
       </c>
       <c r="B76" s="0">
         <v>0</v>
@@ -3993,13 +5988,13 @@
         <v>0</v>
       </c>
       <c r="D76" s="0" t="s">
-        <v>809</v>
+        <v>1472</v>
       </c>
       <c r="E76" s="0"/>
     </row>
     <row r="77">
       <c r="A77" s="0" t="s">
-        <v>740</v>
+        <v>1403</v>
       </c>
       <c r="B77" s="0">
         <v>0</v>
@@ -4008,13 +6003,13 @@
         <v>0</v>
       </c>
       <c r="D77" s="0" t="s">
-        <v>809</v>
+        <v>1472</v>
       </c>
       <c r="E77" s="0"/>
     </row>
     <row r="78">
       <c r="A78" s="0" t="s">
-        <v>741</v>
+        <v>1404</v>
       </c>
       <c r="B78" s="0">
         <v>0</v>
@@ -4023,13 +6018,13 @@
         <v>0</v>
       </c>
       <c r="D78" s="0" t="s">
-        <v>809</v>
+        <v>1472</v>
       </c>
       <c r="E78" s="0"/>
     </row>
     <row r="79">
       <c r="A79" s="0" t="s">
-        <v>742</v>
+        <v>1405</v>
       </c>
       <c r="B79" s="0">
         <v>0</v>
@@ -4038,13 +6033,13 @@
         <v>0</v>
       </c>
       <c r="D79" s="0" t="s">
-        <v>809</v>
+        <v>1472</v>
       </c>
       <c r="E79" s="0"/>
     </row>
     <row r="80">
       <c r="A80" s="0" t="s">
-        <v>743</v>
+        <v>1406</v>
       </c>
       <c r="B80" s="0">
         <v>1</v>
@@ -4053,15 +6048,15 @@
         <v>0</v>
       </c>
       <c r="D80" s="0" t="s">
-        <v>809</v>
+        <v>1472</v>
       </c>
       <c r="E80" s="0" t="s">
-        <v>874</v>
+        <v>1537</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="0" t="s">
-        <v>744</v>
+        <v>1407</v>
       </c>
       <c r="B81" s="0">
         <v>0.69999999999999996</v>
@@ -4070,15 +6065,15 @@
         <v>0</v>
       </c>
       <c r="D81" s="0" t="s">
-        <v>809</v>
+        <v>1472</v>
       </c>
       <c r="E81" s="0" t="s">
-        <v>875</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="0" t="s">
-        <v>745</v>
+        <v>1408</v>
       </c>
       <c r="B82" s="0">
         <v>0.69999999999999996</v>
@@ -4087,15 +6082,15 @@
         <v>0</v>
       </c>
       <c r="D82" s="0" t="s">
-        <v>809</v>
+        <v>1472</v>
       </c>
       <c r="E82" s="0" t="s">
-        <v>876</v>
+        <v>1539</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="0" t="s">
-        <v>746</v>
+        <v>1409</v>
       </c>
       <c r="B83" s="0">
         <v>0.90000000000000002</v>
@@ -4104,15 +6099,15 @@
         <v>0</v>
       </c>
       <c r="D83" s="0" t="s">
-        <v>809</v>
+        <v>1472</v>
       </c>
       <c r="E83" s="0" t="s">
-        <v>877</v>
+        <v>1540</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="0" t="s">
-        <v>747</v>
+        <v>1410</v>
       </c>
       <c r="B84" s="0">
         <v>0.90000000000000002</v>
@@ -4121,15 +6116,15 @@
         <v>0</v>
       </c>
       <c r="D84" s="0" t="s">
-        <v>809</v>
+        <v>1472</v>
       </c>
       <c r="E84" s="0" t="s">
-        <v>878</v>
+        <v>1541</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="0" t="s">
-        <v>748</v>
+        <v>1411</v>
       </c>
       <c r="B85" s="0">
         <v>0.5</v>
@@ -4138,15 +6133,15 @@
         <v>0</v>
       </c>
       <c r="D85" s="0" t="s">
-        <v>809</v>
+        <v>1472</v>
       </c>
       <c r="E85" s="0" t="s">
-        <v>879</v>
+        <v>1542</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="0" t="s">
-        <v>749</v>
+        <v>1412</v>
       </c>
       <c r="B86" s="0">
         <v>0.5</v>
@@ -4155,13 +6150,13 @@
         <v>0</v>
       </c>
       <c r="D86" s="0" t="s">
-        <v>809</v>
+        <v>1472</v>
       </c>
       <c r="E86" s="0"/>
     </row>
     <row r="87">
       <c r="A87" s="0" t="s">
-        <v>750</v>
+        <v>1413</v>
       </c>
       <c r="B87" s="0">
         <v>0.20000000000000001</v>
@@ -4170,13 +6165,13 @@
         <v>0</v>
       </c>
       <c r="D87" s="0" t="s">
-        <v>809</v>
+        <v>1472</v>
       </c>
       <c r="E87" s="0"/>
     </row>
     <row r="88">
       <c r="A88" s="0" t="s">
-        <v>751</v>
+        <v>1414</v>
       </c>
       <c r="B88" s="0">
         <v>0</v>
@@ -4185,13 +6180,13 @@
         <v>0</v>
       </c>
       <c r="D88" s="0" t="s">
-        <v>809</v>
+        <v>1472</v>
       </c>
       <c r="E88" s="0"/>
     </row>
     <row r="89">
       <c r="A89" s="0" t="s">
-        <v>752</v>
+        <v>1415</v>
       </c>
       <c r="B89" s="0">
         <v>1</v>
@@ -4200,13 +6195,13 @@
         <v>0</v>
       </c>
       <c r="D89" s="0" t="s">
-        <v>809</v>
+        <v>1472</v>
       </c>
       <c r="E89" s="0"/>
     </row>
     <row r="90">
       <c r="A90" s="0" t="s">
-        <v>753</v>
+        <v>1416</v>
       </c>
       <c r="B90" s="0">
         <v>0</v>
@@ -4215,13 +6210,13 @@
         <v>0</v>
       </c>
       <c r="D90" s="0" t="s">
-        <v>809</v>
+        <v>1472</v>
       </c>
       <c r="E90" s="0"/>
     </row>
     <row r="91">
       <c r="A91" s="0" t="s">
-        <v>754</v>
+        <v>1417</v>
       </c>
       <c r="B91" s="0">
         <v>0.029999999999999999</v>
@@ -4230,13 +6225,13 @@
         <v>0</v>
       </c>
       <c r="D91" s="0" t="s">
-        <v>809</v>
+        <v>1472</v>
       </c>
       <c r="E91" s="0"/>
     </row>
     <row r="92">
       <c r="A92" s="0" t="s">
-        <v>755</v>
+        <v>1418</v>
       </c>
       <c r="B92" s="0">
         <v>0</v>
@@ -4245,13 +6240,13 @@
         <v>0</v>
       </c>
       <c r="D92" s="0" t="s">
-        <v>809</v>
+        <v>1472</v>
       </c>
       <c r="E92" s="0"/>
     </row>
     <row r="93">
       <c r="A93" s="0" t="s">
-        <v>756</v>
+        <v>1419</v>
       </c>
       <c r="B93" s="0">
         <v>0.5</v>
@@ -4260,13 +6255,13 @@
         <v>0</v>
       </c>
       <c r="D93" s="0" t="s">
-        <v>809</v>
+        <v>1472</v>
       </c>
       <c r="E93" s="0"/>
     </row>
     <row r="94">
       <c r="A94" s="0" t="s">
-        <v>757</v>
+        <v>1420</v>
       </c>
       <c r="B94" s="0">
         <v>1</v>
@@ -4275,13 +6270,13 @@
         <v>0</v>
       </c>
       <c r="D94" s="0" t="s">
-        <v>809</v>
+        <v>1472</v>
       </c>
       <c r="E94" s="0"/>
     </row>
     <row r="95">
       <c r="A95" s="0" t="s">
-        <v>758</v>
+        <v>1421</v>
       </c>
       <c r="B95" s="0">
         <v>0.20000000000000001</v>
@@ -4290,13 +6285,13 @@
         <v>0</v>
       </c>
       <c r="D95" s="0" t="s">
-        <v>809</v>
+        <v>1472</v>
       </c>
       <c r="E95" s="0"/>
     </row>
     <row r="96">
       <c r="A96" s="0" t="s">
-        <v>759</v>
+        <v>1422</v>
       </c>
       <c r="B96" s="0">
         <v>0.94999999999999996</v>
@@ -4305,13 +6300,13 @@
         <v>0</v>
       </c>
       <c r="D96" s="0" t="s">
-        <v>809</v>
+        <v>1472</v>
       </c>
       <c r="E96" s="0"/>
     </row>
     <row r="97">
       <c r="A97" s="0" t="s">
-        <v>760</v>
+        <v>1423</v>
       </c>
       <c r="B97" s="0">
         <v>0.90000000000000002</v>
@@ -4320,13 +6315,13 @@
         <v>0</v>
       </c>
       <c r="D97" s="0" t="s">
-        <v>809</v>
+        <v>1472</v>
       </c>
       <c r="E97" s="0"/>
     </row>
     <row r="98">
       <c r="A98" s="0" t="s">
-        <v>761</v>
+        <v>1424</v>
       </c>
       <c r="B98" s="0">
         <v>0.14999999999999999</v>
@@ -4335,28 +6330,28 @@
         <v>0</v>
       </c>
       <c r="D98" s="0" t="s">
-        <v>809</v>
+        <v>1472</v>
       </c>
       <c r="E98" s="0"/>
     </row>
     <row r="99">
       <c r="A99" s="0" t="s">
-        <v>762</v>
+        <v>1425</v>
       </c>
       <c r="B99" s="0">
-        <v>0</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="C99" s="0">
         <v>0</v>
       </c>
       <c r="D99" s="0" t="s">
-        <v>809</v>
+        <v>1472</v>
       </c>
       <c r="E99" s="0"/>
     </row>
     <row r="100">
       <c r="A100" s="0" t="s">
-        <v>763</v>
+        <v>1426</v>
       </c>
       <c r="B100" s="0">
         <v>0.69999999999999996</v>
@@ -4365,13 +6360,13 @@
         <v>0</v>
       </c>
       <c r="D100" s="0" t="s">
-        <v>809</v>
+        <v>1472</v>
       </c>
       <c r="E100" s="0"/>
     </row>
     <row r="101">
       <c r="A101" s="0" t="s">
-        <v>764</v>
+        <v>1427</v>
       </c>
       <c r="B101" s="0">
         <v>0.29999999999999999</v>
@@ -4380,13 +6375,13 @@
         <v>0</v>
       </c>
       <c r="D101" s="0" t="s">
-        <v>809</v>
+        <v>1472</v>
       </c>
       <c r="E101" s="0"/>
     </row>
     <row r="102">
       <c r="A102" s="0" t="s">
-        <v>765</v>
+        <v>1428</v>
       </c>
       <c r="B102" s="0">
         <v>0.59999999999999998</v>
@@ -4395,13 +6390,13 @@
         <v>0</v>
       </c>
       <c r="D102" s="0" t="s">
-        <v>809</v>
+        <v>1472</v>
       </c>
       <c r="E102" s="0"/>
     </row>
     <row r="103">
       <c r="A103" s="0" t="s">
-        <v>766</v>
+        <v>1429</v>
       </c>
       <c r="B103" s="0">
         <v>0</v>
@@ -4410,13 +6405,13 @@
         <v>0</v>
       </c>
       <c r="D103" s="0" t="s">
-        <v>809</v>
+        <v>1472</v>
       </c>
       <c r="E103" s="0"/>
     </row>
     <row r="104">
       <c r="A104" s="0" t="s">
-        <v>767</v>
+        <v>1430</v>
       </c>
       <c r="B104" s="0">
         <v>0.40000000000000002</v>
@@ -4425,13 +6420,13 @@
         <v>0</v>
       </c>
       <c r="D104" s="0" t="s">
-        <v>809</v>
+        <v>1472</v>
       </c>
       <c r="E104" s="0"/>
     </row>
     <row r="105">
       <c r="A105" s="0" t="s">
-        <v>768</v>
+        <v>1431</v>
       </c>
       <c r="B105" s="0">
         <v>0.10000000000000001</v>
@@ -4440,13 +6435,13 @@
         <v>0</v>
       </c>
       <c r="D105" s="0" t="s">
-        <v>809</v>
+        <v>1472</v>
       </c>
       <c r="E105" s="0"/>
     </row>
     <row r="106">
       <c r="A106" s="0" t="s">
-        <v>769</v>
+        <v>1432</v>
       </c>
       <c r="B106" s="0">
         <v>0.5</v>
@@ -4455,13 +6450,13 @@
         <v>0</v>
       </c>
       <c r="D106" s="0" t="s">
-        <v>809</v>
+        <v>1472</v>
       </c>
       <c r="E106" s="0"/>
     </row>
     <row r="107">
       <c r="A107" s="0" t="s">
-        <v>770</v>
+        <v>1433</v>
       </c>
       <c r="B107" s="0">
         <v>1</v>
@@ -4470,13 +6465,13 @@
         <v>0</v>
       </c>
       <c r="D107" s="0" t="s">
-        <v>809</v>
+        <v>1472</v>
       </c>
       <c r="E107" s="0"/>
     </row>
     <row r="108">
       <c r="A108" s="0" t="s">
-        <v>771</v>
+        <v>1434</v>
       </c>
       <c r="B108" s="0">
         <v>1</v>
@@ -4485,13 +6480,13 @@
         <v>0</v>
       </c>
       <c r="D108" s="0" t="s">
-        <v>809</v>
+        <v>1472</v>
       </c>
       <c r="E108" s="0"/>
     </row>
     <row r="109">
       <c r="A109" s="0" t="s">
-        <v>772</v>
+        <v>1435</v>
       </c>
       <c r="B109" s="0">
         <v>25</v>
@@ -4500,13 +6495,13 @@
         <v>0</v>
       </c>
       <c r="D109" s="0" t="s">
-        <v>809</v>
+        <v>1472</v>
       </c>
       <c r="E109" s="0"/>
     </row>
     <row r="110">
       <c r="A110" s="0" t="s">
-        <v>773</v>
+        <v>1436</v>
       </c>
       <c r="B110" s="0">
         <v>1.1000000000000001</v>
@@ -4515,28 +6510,28 @@
         <v>0</v>
       </c>
       <c r="D110" s="0" t="s">
-        <v>809</v>
+        <v>1472</v>
       </c>
       <c r="E110" s="0"/>
     </row>
     <row r="111">
       <c r="A111" s="0" t="s">
-        <v>774</v>
+        <v>1437</v>
       </c>
       <c r="B111" s="0">
-        <v>1</v>
+        <v>1.2</v>
       </c>
       <c r="C111" s="0">
         <v>0</v>
       </c>
       <c r="D111" s="0" t="s">
-        <v>809</v>
+        <v>1472</v>
       </c>
       <c r="E111" s="0"/>
     </row>
     <row r="112">
       <c r="A112" s="0" t="s">
-        <v>775</v>
+        <v>1438</v>
       </c>
       <c r="B112" s="0">
         <v>0.5</v>
@@ -4545,13 +6540,13 @@
         <v>0</v>
       </c>
       <c r="D112" s="0" t="s">
-        <v>809</v>
+        <v>1472</v>
       </c>
       <c r="E112" s="0"/>
     </row>
     <row r="113">
       <c r="A113" s="0" t="s">
-        <v>776</v>
+        <v>1439</v>
       </c>
       <c r="B113" s="0">
         <v>3</v>
@@ -4560,13 +6555,13 @@
         <v>0</v>
       </c>
       <c r="D113" s="0" t="s">
-        <v>809</v>
+        <v>1472</v>
       </c>
       <c r="E113" s="0"/>
     </row>
     <row r="114">
       <c r="A114" s="0" t="s">
-        <v>777</v>
+        <v>1440</v>
       </c>
       <c r="B114" s="0">
         <v>0.5</v>
@@ -4575,13 +6570,13 @@
         <v>0</v>
       </c>
       <c r="D114" s="0" t="s">
-        <v>809</v>
+        <v>1472</v>
       </c>
       <c r="E114" s="0"/>
     </row>
     <row r="115">
       <c r="A115" s="0" t="s">
-        <v>778</v>
+        <v>1441</v>
       </c>
       <c r="B115" s="0">
         <v>4</v>
@@ -4590,13 +6585,13 @@
         <v>0</v>
       </c>
       <c r="D115" s="0" t="s">
-        <v>809</v>
+        <v>1472</v>
       </c>
       <c r="E115" s="0"/>
     </row>
     <row r="116">
       <c r="A116" s="0" t="s">
-        <v>779</v>
+        <v>1442</v>
       </c>
       <c r="B116" s="0">
         <v>2</v>
@@ -4605,13 +6600,13 @@
         <v>0</v>
       </c>
       <c r="D116" s="0" t="s">
-        <v>809</v>
+        <v>1472</v>
       </c>
       <c r="E116" s="0"/>
     </row>
     <row r="117">
       <c r="A117" s="0" t="s">
-        <v>780</v>
+        <v>1443</v>
       </c>
       <c r="B117" s="0">
         <v>0.40000000000000002</v>
@@ -4620,13 +6615,13 @@
         <v>0</v>
       </c>
       <c r="D117" s="0" t="s">
-        <v>809</v>
+        <v>1472</v>
       </c>
       <c r="E117" s="0"/>
     </row>
     <row r="118">
       <c r="A118" s="0" t="s">
-        <v>781</v>
+        <v>1444</v>
       </c>
       <c r="B118" s="0">
         <v>0.5</v>
@@ -4635,13 +6630,13 @@
         <v>0</v>
       </c>
       <c r="D118" s="0" t="s">
-        <v>809</v>
+        <v>1472</v>
       </c>
       <c r="E118" s="0"/>
     </row>
     <row r="119">
       <c r="A119" s="0" t="s">
-        <v>782</v>
+        <v>1445</v>
       </c>
       <c r="B119" s="0">
         <v>0.5</v>
@@ -4650,13 +6645,13 @@
         <v>0</v>
       </c>
       <c r="D119" s="0" t="s">
-        <v>809</v>
+        <v>1472</v>
       </c>
       <c r="E119" s="0"/>
     </row>
     <row r="120">
       <c r="A120" s="0" t="s">
-        <v>783</v>
+        <v>1446</v>
       </c>
       <c r="B120" s="0">
         <v>0.5</v>
@@ -4665,15 +6660,15 @@
         <v>0</v>
       </c>
       <c r="D120" s="0" t="s">
-        <v>809</v>
+        <v>1472</v>
       </c>
       <c r="E120" s="0" t="s">
-        <v>880</v>
+        <v>1543</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="0" t="s">
-        <v>784</v>
+        <v>1447</v>
       </c>
       <c r="B121" s="0">
         <v>0.5</v>
@@ -4682,15 +6677,15 @@
         <v>0</v>
       </c>
       <c r="D121" s="0" t="s">
-        <v>809</v>
+        <v>1472</v>
       </c>
       <c r="E121" s="0" t="s">
-        <v>881</v>
+        <v>1544</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="0" t="s">
-        <v>785</v>
+        <v>1448</v>
       </c>
       <c r="B122" s="0">
         <v>0.10000000000000001</v>
@@ -4699,15 +6694,15 @@
         <v>0</v>
       </c>
       <c r="D122" s="0" t="s">
-        <v>809</v>
+        <v>1472</v>
       </c>
       <c r="E122" s="0" t="s">
-        <v>882</v>
+        <v>1545</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="0" t="s">
-        <v>786</v>
+        <v>1449</v>
       </c>
       <c r="B123" s="0">
         <v>0.59999999999999998</v>
@@ -4716,15 +6711,15 @@
         <v>0</v>
       </c>
       <c r="D123" s="0" t="s">
-        <v>809</v>
+        <v>1472</v>
       </c>
       <c r="E123" s="0" t="s">
-        <v>883</v>
+        <v>1546</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="0" t="s">
-        <v>787</v>
+        <v>1450</v>
       </c>
       <c r="B124" s="0">
         <v>0.40000000000000002</v>
@@ -4733,13 +6728,13 @@
         <v>0</v>
       </c>
       <c r="D124" s="0" t="s">
-        <v>809</v>
+        <v>1472</v>
       </c>
       <c r="E124" s="0"/>
     </row>
     <row r="125">
       <c r="A125" s="0" t="s">
-        <v>788</v>
+        <v>1451</v>
       </c>
       <c r="B125" s="0">
         <v>0.20000000000000001</v>
@@ -4748,13 +6743,13 @@
         <v>0</v>
       </c>
       <c r="D125" s="0" t="s">
-        <v>809</v>
+        <v>1472</v>
       </c>
       <c r="E125" s="0"/>
     </row>
     <row r="126">
       <c r="A126" s="0" t="s">
-        <v>789</v>
+        <v>1452</v>
       </c>
       <c r="B126" s="0">
         <v>0</v>
@@ -4763,13 +6758,13 @@
         <v>0</v>
       </c>
       <c r="D126" s="0" t="s">
-        <v>809</v>
+        <v>1472</v>
       </c>
       <c r="E126" s="0"/>
     </row>
     <row r="127">
       <c r="A127" s="0" t="s">
-        <v>790</v>
+        <v>1453</v>
       </c>
       <c r="B127" s="0">
         <v>2.5</v>
@@ -4778,13 +6773,13 @@
         <v>0</v>
       </c>
       <c r="D127" s="0" t="s">
-        <v>809</v>
+        <v>1472</v>
       </c>
       <c r="E127" s="0"/>
     </row>
     <row r="128">
       <c r="A128" s="0" t="s">
-        <v>791</v>
+        <v>1454</v>
       </c>
       <c r="B128" s="0">
         <v>0.5</v>
@@ -4793,13 +6788,13 @@
         <v>0</v>
       </c>
       <c r="D128" s="0" t="s">
-        <v>809</v>
+        <v>1472</v>
       </c>
       <c r="E128" s="0"/>
     </row>
     <row r="129">
       <c r="A129" s="0" t="s">
-        <v>792</v>
+        <v>1455</v>
       </c>
       <c r="B129" s="0">
         <v>0.5</v>
@@ -4808,13 +6803,13 @@
         <v>0</v>
       </c>
       <c r="D129" s="0" t="s">
-        <v>809</v>
+        <v>1472</v>
       </c>
       <c r="E129" s="0"/>
     </row>
     <row r="130">
       <c r="A130" s="0" t="s">
-        <v>793</v>
+        <v>1456</v>
       </c>
       <c r="B130" s="0">
         <v>0.5</v>
@@ -4823,13 +6818,13 @@
         <v>0</v>
       </c>
       <c r="D130" s="0" t="s">
-        <v>809</v>
+        <v>1472</v>
       </c>
       <c r="E130" s="0"/>
     </row>
     <row r="131">
       <c r="A131" s="0" t="s">
-        <v>794</v>
+        <v>1457</v>
       </c>
       <c r="B131" s="0">
         <v>0.5</v>
@@ -4838,13 +6833,13 @@
         <v>0</v>
       </c>
       <c r="D131" s="0" t="s">
-        <v>809</v>
+        <v>1472</v>
       </c>
       <c r="E131" s="0"/>
     </row>
     <row r="132">
       <c r="A132" s="0" t="s">
-        <v>795</v>
+        <v>1458</v>
       </c>
       <c r="B132" s="0">
         <v>1</v>
@@ -4853,13 +6848,13 @@
         <v>0</v>
       </c>
       <c r="D132" s="0" t="s">
-        <v>809</v>
+        <v>1472</v>
       </c>
       <c r="E132" s="0"/>
     </row>
     <row r="133">
       <c r="A133" s="0" t="s">
-        <v>796</v>
+        <v>1459</v>
       </c>
       <c r="B133" s="0">
         <v>0.90000000000000002</v>
@@ -4868,13 +6863,13 @@
         <v>0</v>
       </c>
       <c r="D133" s="0" t="s">
-        <v>809</v>
+        <v>1472</v>
       </c>
       <c r="E133" s="0"/>
     </row>
     <row r="134">
       <c r="A134" s="0" t="s">
-        <v>797</v>
+        <v>1460</v>
       </c>
       <c r="B134" s="0">
         <v>1</v>
@@ -4883,13 +6878,13 @@
         <v>0</v>
       </c>
       <c r="D134" s="0" t="s">
-        <v>809</v>
+        <v>1472</v>
       </c>
       <c r="E134" s="0"/>
     </row>
     <row r="135">
       <c r="A135" s="0" t="s">
-        <v>798</v>
+        <v>1461</v>
       </c>
       <c r="B135" s="0">
         <v>0</v>
@@ -4898,10 +6893,10 @@
         <v>1</v>
       </c>
       <c r="D135" s="0" t="s">
-        <v>809</v>
+        <v>1472</v>
       </c>
       <c r="E135" s="0" t="s">
-        <v>884</v>
+        <v>1547</v>
       </c>
     </row>
   </sheetData>

</xml_diff>